<commit_message>
Here is my CSRT code
</commit_message>
<xml_diff>
--- a/MACH1.xlsx
+++ b/MACH1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C279"/>
+  <dimension ref="A1:C280"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Frames</t>
+          <t>Frame</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -445,10 +445,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1187</v>
+        <v>1197</v>
       </c>
       <c r="C2" t="n">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3">
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1171</v>
+        <v>1186</v>
       </c>
       <c r="C3" t="n">
-        <v>401</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4">
@@ -471,10 +471,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1146</v>
+        <v>1170</v>
       </c>
       <c r="C4" t="n">
-        <v>422</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5">
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1119</v>
+        <v>1145</v>
       </c>
       <c r="C5" t="n">
-        <v>448</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1092</v>
+        <v>1117</v>
       </c>
       <c r="C6" t="n">
-        <v>481</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1066</v>
+        <v>1089</v>
       </c>
       <c r="C7" t="n">
-        <v>516</v>
+        <v>483</v>
       </c>
     </row>
     <row r="8">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1044</v>
+        <v>1063</v>
       </c>
       <c r="C8" t="n">
-        <v>553</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9">
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1030</v>
+        <v>1043</v>
       </c>
       <c r="C9" t="n">
-        <v>584</v>
+        <v>555</v>
       </c>
     </row>
     <row r="10">
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C10" t="n">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="11">
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="C11" t="n">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="12">
@@ -575,10 +575,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="C12" t="n">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="13">
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1020</v>
+        <v>1024</v>
       </c>
       <c r="C13" t="n">
-        <v>585</v>
+        <v>590</v>
       </c>
     </row>
     <row r="14">
@@ -604,7 +604,7 @@
         <v>1018</v>
       </c>
       <c r="C14" t="n">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="15">
@@ -614,10 +614,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C15" t="n">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="16">
@@ -627,10 +627,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="C16" t="n">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="17">
@@ -640,10 +640,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C17" t="n">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="18">
@@ -653,10 +653,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="C18" t="n">
-        <v>577</v>
+        <v>583</v>
       </c>
     </row>
     <row r="19">
@@ -666,10 +666,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="C19" t="n">
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="20">
@@ -679,10 +679,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C20" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="21">
@@ -692,10 +692,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="C21" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="22">
@@ -705,10 +705,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="C22" t="n">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="23">
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C23" t="n">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="24">
@@ -731,10 +731,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C24" t="n">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="25">
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1007</v>
+        <v>992</v>
       </c>
       <c r="C25" t="n">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="26">
@@ -757,10 +757,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1034</v>
+        <v>1006</v>
       </c>
       <c r="C26" t="n">
-        <v>562</v>
+        <v>579</v>
       </c>
     </row>
     <row r="27">
@@ -770,10 +770,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1056</v>
+        <v>1031</v>
       </c>
       <c r="C27" t="n">
-        <v>528</v>
+        <v>564</v>
       </c>
     </row>
     <row r="28">
@@ -783,10 +783,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1082</v>
+        <v>1053</v>
       </c>
       <c r="C28" t="n">
-        <v>495</v>
+        <v>531</v>
       </c>
     </row>
     <row r="29">
@@ -796,10 +796,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1110</v>
+        <v>1080</v>
       </c>
       <c r="C29" t="n">
-        <v>459</v>
+        <v>498</v>
       </c>
     </row>
     <row r="30">
@@ -809,10 +809,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1139</v>
+        <v>1107</v>
       </c>
       <c r="C30" t="n">
-        <v>426</v>
+        <v>463</v>
       </c>
     </row>
     <row r="31">
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1164</v>
+        <v>1136</v>
       </c>
       <c r="C31" t="n">
-        <v>400</v>
+        <v>429</v>
       </c>
     </row>
     <row r="32">
@@ -835,10 +835,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1186</v>
+        <v>1163</v>
       </c>
       <c r="C32" t="n">
-        <v>383</v>
+        <v>402</v>
       </c>
     </row>
     <row r="33">
@@ -848,10 +848,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1194</v>
+        <v>1184</v>
       </c>
       <c r="C33" t="n">
-        <v>374</v>
+        <v>385</v>
       </c>
     </row>
     <row r="34">
@@ -861,10 +861,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1196</v>
+        <v>1193</v>
       </c>
       <c r="C34" t="n">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35">
@@ -874,10 +874,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="C35" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36">
@@ -887,10 +887,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="C36" t="n">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="37">
@@ -900,10 +900,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C37" t="n">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="38">
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="C38" t="n">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="39">
@@ -926,10 +926,10 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1201</v>
+        <v>1194</v>
       </c>
       <c r="C39" t="n">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="40">
@@ -939,10 +939,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1226</v>
+        <v>1198</v>
       </c>
       <c r="C40" t="n">
-        <v>406</v>
+        <v>379</v>
       </c>
     </row>
     <row r="41">
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>1256</v>
+        <v>1225</v>
       </c>
       <c r="C41" t="n">
-        <v>436</v>
+        <v>407</v>
       </c>
     </row>
     <row r="42">
@@ -965,10 +965,10 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>1275</v>
+        <v>1255</v>
       </c>
       <c r="C42" t="n">
-        <v>467</v>
+        <v>437</v>
       </c>
     </row>
     <row r="43">
@@ -978,10 +978,10 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>1283</v>
+        <v>1275</v>
       </c>
       <c r="C43" t="n">
-        <v>505</v>
+        <v>469</v>
       </c>
     </row>
     <row r="44">
@@ -991,10 +991,10 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1278</v>
+        <v>1283</v>
       </c>
       <c r="C44" t="n">
-        <v>539</v>
+        <v>506</v>
       </c>
     </row>
     <row r="45">
@@ -1004,10 +1004,10 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1262</v>
+        <v>1278</v>
       </c>
       <c r="C45" t="n">
-        <v>574</v>
+        <v>541</v>
       </c>
     </row>
     <row r="46">
@@ -1017,10 +1017,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1234</v>
+        <v>1261</v>
       </c>
       <c r="C46" t="n">
-        <v>603</v>
+        <v>576</v>
       </c>
     </row>
     <row r="47">
@@ -1030,10 +1030,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1202</v>
+        <v>1233</v>
       </c>
       <c r="C47" t="n">
-        <v>621</v>
+        <v>605</v>
       </c>
     </row>
     <row r="48">
@@ -1043,10 +1043,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1176</v>
+        <v>1201</v>
       </c>
       <c r="C48" t="n">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="49">
@@ -1056,10 +1056,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1166</v>
+        <v>1174</v>
       </c>
       <c r="C49" t="n">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="50">
@@ -1069,10 +1069,10 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="C50" t="n">
-        <v>615</v>
+        <v>620</v>
       </c>
     </row>
     <row r="51">
@@ -1085,7 +1085,7 @@
         <v>1166</v>
       </c>
       <c r="C51" t="n">
-        <v>614</v>
+        <v>618</v>
       </c>
     </row>
     <row r="52">
@@ -1098,7 +1098,7 @@
         <v>1166</v>
       </c>
       <c r="C52" t="n">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="53">
@@ -1108,10 +1108,10 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C53" t="n">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="54">
@@ -1124,7 +1124,7 @@
         <v>1166</v>
       </c>
       <c r="C54" t="n">
-        <v>613</v>
+        <v>617</v>
       </c>
     </row>
     <row r="55">
@@ -1137,7 +1137,7 @@
         <v>1167</v>
       </c>
       <c r="C55" t="n">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="56">
@@ -1150,7 +1150,7 @@
         <v>1166</v>
       </c>
       <c r="C56" t="n">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="57">
@@ -1163,7 +1163,7 @@
         <v>1167</v>
       </c>
       <c r="C57" t="n">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="58">
@@ -1176,7 +1176,7 @@
         <v>1166</v>
       </c>
       <c r="C58" t="n">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="59">
@@ -1186,10 +1186,10 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C59" t="n">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="60">
@@ -1199,10 +1199,10 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="C60" t="n">
-        <v>614</v>
+        <v>618</v>
       </c>
     </row>
     <row r="61">
@@ -1215,7 +1215,7 @@
         <v>1166</v>
       </c>
       <c r="C61" t="n">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="62">
@@ -1225,10 +1225,10 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C62" t="n">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="63">
@@ -1238,10 +1238,10 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="C63" t="n">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="64">
@@ -1254,7 +1254,7 @@
         <v>1166</v>
       </c>
       <c r="C64" t="n">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="65">
@@ -1267,7 +1267,7 @@
         <v>1166</v>
       </c>
       <c r="C65" t="n">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="66">
@@ -1280,7 +1280,7 @@
         <v>1166</v>
       </c>
       <c r="C66" t="n">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="67">
@@ -1293,7 +1293,7 @@
         <v>1166</v>
       </c>
       <c r="C67" t="n">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="68">
@@ -1306,7 +1306,7 @@
         <v>1166</v>
       </c>
       <c r="C68" t="n">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="69">
@@ -1316,10 +1316,10 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="C69" t="n">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="70">
@@ -1329,10 +1329,10 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1196</v>
+        <v>1169</v>
       </c>
       <c r="C70" t="n">
-        <v>610</v>
+        <v>616</v>
       </c>
     </row>
     <row r="71">
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1226</v>
+        <v>1195</v>
       </c>
       <c r="C71" t="n">
-        <v>594</v>
+        <v>613</v>
       </c>
     </row>
     <row r="72">
@@ -1355,10 +1355,10 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>1254</v>
+        <v>1226</v>
       </c>
       <c r="C72" t="n">
-        <v>565</v>
+        <v>597</v>
       </c>
     </row>
     <row r="73">
@@ -1368,10 +1368,10 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1275</v>
+        <v>1253</v>
       </c>
       <c r="C73" t="n">
-        <v>534</v>
+        <v>570</v>
       </c>
     </row>
     <row r="74">
@@ -1381,10 +1381,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1284</v>
+        <v>1274</v>
       </c>
       <c r="C74" t="n">
-        <v>502</v>
+        <v>537</v>
       </c>
     </row>
     <row r="75">
@@ -1394,10 +1394,10 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1277</v>
+        <v>1283</v>
       </c>
       <c r="C75" t="n">
-        <v>469</v>
+        <v>506</v>
       </c>
     </row>
     <row r="76">
@@ -1407,10 +1407,10 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1254</v>
+        <v>1277</v>
       </c>
       <c r="C76" t="n">
-        <v>437</v>
+        <v>472</v>
       </c>
     </row>
     <row r="77">
@@ -1420,10 +1420,10 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>1222</v>
+        <v>1254</v>
       </c>
       <c r="C77" t="n">
-        <v>409</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78">
@@ -1433,10 +1433,10 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>1194</v>
+        <v>1222</v>
       </c>
       <c r="C78" t="n">
-        <v>382</v>
+        <v>410</v>
       </c>
     </row>
     <row r="79">
@@ -1446,10 +1446,10 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>1186</v>
+        <v>1193</v>
       </c>
       <c r="C79" t="n">
-        <v>371</v>
+        <v>385</v>
       </c>
     </row>
     <row r="80">
@@ -1459,10 +1459,10 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C80" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="81">
@@ -1475,7 +1475,7 @@
         <v>1187</v>
       </c>
       <c r="C81" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="82">
@@ -1485,10 +1485,10 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="C82" t="n">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83">
@@ -1498,10 +1498,10 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C83" t="n">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="84">
@@ -1511,10 +1511,10 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C84" t="n">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="85">
@@ -1524,10 +1524,10 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C85" t="n">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="86">
@@ -1537,10 +1537,10 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="C86" t="n">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="87">
@@ -1550,10 +1550,10 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C87" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="88">
@@ -1563,10 +1563,10 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C88" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="89">
@@ -1576,10 +1576,10 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C89" t="n">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="90">
@@ -1589,10 +1589,10 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C90" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="91">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C91" t="n">
         <v>374</v>
@@ -1615,10 +1615,10 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>1191</v>
+        <v>1188</v>
       </c>
       <c r="C92" t="n">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="93">
@@ -1628,10 +1628,10 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="C93" t="n">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="94">
@@ -1641,10 +1641,10 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C94" t="n">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="95">
@@ -1654,10 +1654,10 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>1186</v>
+        <v>1188</v>
       </c>
       <c r="C95" t="n">
-        <v>369</v>
+        <v>376</v>
       </c>
     </row>
     <row r="96">
@@ -1667,10 +1667,10 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>1158</v>
+        <v>1185</v>
       </c>
       <c r="C96" t="n">
-        <v>345</v>
+        <v>371</v>
       </c>
     </row>
     <row r="97">
@@ -1680,10 +1680,10 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>1120</v>
+        <v>1156</v>
       </c>
       <c r="C97" t="n">
-        <v>318</v>
+        <v>348</v>
       </c>
     </row>
     <row r="98">
@@ -1693,10 +1693,10 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>1082</v>
+        <v>1119</v>
       </c>
       <c r="C98" t="n">
-        <v>296</v>
+        <v>319</v>
       </c>
     </row>
     <row r="99">
@@ -1706,10 +1706,10 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>1037</v>
+        <v>1081</v>
       </c>
       <c r="C99" t="n">
-        <v>274</v>
+        <v>298</v>
       </c>
     </row>
     <row r="100">
@@ -1719,10 +1719,10 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>990</v>
+        <v>1036</v>
       </c>
       <c r="C100" t="n">
-        <v>257</v>
+        <v>276</v>
       </c>
     </row>
     <row r="101">
@@ -1732,10 +1732,10 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>944</v>
+        <v>990</v>
       </c>
       <c r="C101" t="n">
-        <v>244</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102">
@@ -1745,10 +1745,10 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>897</v>
+        <v>945</v>
       </c>
       <c r="C102" t="n">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="103">
@@ -1758,10 +1758,10 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>854</v>
+        <v>897</v>
       </c>
       <c r="C103" t="n">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104">
@@ -1771,10 +1771,10 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>829</v>
+        <v>853</v>
       </c>
       <c r="C104" t="n">
-        <v>213</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105">
@@ -1784,10 +1784,10 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>837</v>
+        <v>827</v>
       </c>
       <c r="C105" t="n">
-        <v>183</v>
+        <v>216</v>
       </c>
     </row>
     <row r="106">
@@ -1797,10 +1797,10 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>879</v>
+        <v>836</v>
       </c>
       <c r="C106" t="n">
-        <v>158</v>
+        <v>186</v>
       </c>
     </row>
     <row r="107">
@@ -1810,10 +1810,10 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>942</v>
+        <v>879</v>
       </c>
       <c r="C107" t="n">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="108">
@@ -1823,10 +1823,10 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>990</v>
+        <v>941</v>
       </c>
       <c r="C108" t="n">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="109">
@@ -1836,10 +1836,10 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>1011</v>
+        <v>990</v>
       </c>
       <c r="C109" t="n">
-        <v>208</v>
+        <v>178</v>
       </c>
     </row>
     <row r="110">
@@ -1849,10 +1849,10 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="C110" t="n">
-        <v>243</v>
+        <v>210</v>
       </c>
     </row>
     <row r="111">
@@ -1862,10 +1862,10 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>989</v>
+        <v>1007</v>
       </c>
       <c r="C111" t="n">
-        <v>278</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112">
@@ -1875,10 +1875,10 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>962</v>
+        <v>988</v>
       </c>
       <c r="C112" t="n">
-        <v>313</v>
+        <v>280</v>
       </c>
     </row>
     <row r="113">
@@ -1888,10 +1888,10 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>930</v>
+        <v>961</v>
       </c>
       <c r="C113" t="n">
-        <v>348</v>
+        <v>315</v>
       </c>
     </row>
     <row r="114">
@@ -1901,10 +1901,10 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>896</v>
+        <v>928</v>
       </c>
       <c r="C114" t="n">
-        <v>387</v>
+        <v>351</v>
       </c>
     </row>
     <row r="115">
@@ -1914,10 +1914,10 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>862</v>
+        <v>895</v>
       </c>
       <c r="C115" t="n">
-        <v>428</v>
+        <v>390</v>
       </c>
     </row>
     <row r="116">
@@ -1927,10 +1927,10 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>827</v>
+        <v>862</v>
       </c>
       <c r="C116" t="n">
-        <v>463</v>
+        <v>429</v>
       </c>
     </row>
     <row r="117">
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>792</v>
+        <v>827</v>
       </c>
       <c r="C117" t="n">
-        <v>488</v>
+        <v>465</v>
       </c>
     </row>
     <row r="118">
@@ -1953,10 +1953,10 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>753</v>
+        <v>792</v>
       </c>
       <c r="C118" t="n">
-        <v>495</v>
+        <v>488</v>
       </c>
     </row>
     <row r="119">
@@ -1966,10 +1966,10 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>715</v>
+        <v>753</v>
       </c>
       <c r="C119" t="n">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="120">
@@ -1979,10 +1979,10 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>680</v>
+        <v>714</v>
       </c>
       <c r="C120" t="n">
-        <v>518</v>
+        <v>507</v>
       </c>
     </row>
     <row r="121">
@@ -1992,10 +1992,10 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>646</v>
+        <v>680</v>
       </c>
       <c r="C121" t="n">
-        <v>534</v>
+        <v>520</v>
       </c>
     </row>
     <row r="122">
@@ -2005,10 +2005,10 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>615</v>
+        <v>647</v>
       </c>
       <c r="C122" t="n">
-        <v>550</v>
+        <v>536</v>
       </c>
     </row>
     <row r="123">
@@ -2018,10 +2018,10 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>586</v>
+        <v>615</v>
       </c>
       <c r="C123" t="n">
-        <v>569</v>
+        <v>553</v>
       </c>
     </row>
     <row r="124">
@@ -2031,10 +2031,10 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>564</v>
+        <v>585</v>
       </c>
       <c r="C124" t="n">
-        <v>582</v>
+        <v>572</v>
       </c>
     </row>
     <row r="125">
@@ -2044,10 +2044,10 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>554</v>
+        <v>562</v>
       </c>
       <c r="C125" t="n">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="126">
@@ -2057,10 +2057,10 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C126" t="n">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="127">
@@ -2070,10 +2070,10 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C127" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="128">
@@ -2083,10 +2083,10 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C128" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="129">
@@ -2096,10 +2096,10 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C129" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="130">
@@ -2109,10 +2109,10 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C130" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="131">
@@ -2122,10 +2122,10 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C131" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="132">
@@ -2135,10 +2135,10 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C132" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="133">
@@ -2148,10 +2148,10 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C133" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="134">
@@ -2161,10 +2161,10 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C134" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="135">
@@ -2174,10 +2174,10 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C135" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="136">
@@ -2187,10 +2187,10 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C136" t="n">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="137">
@@ -2200,10 +2200,10 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C137" t="n">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="138">
@@ -2213,10 +2213,10 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C138" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="139">
@@ -2226,10 +2226,10 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C139" t="n">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="140">
@@ -2239,10 +2239,10 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C140" t="n">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="141">
@@ -2252,10 +2252,10 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C141" t="n">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="142">
@@ -2265,10 +2265,10 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C142" t="n">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="143">
@@ -2278,10 +2278,10 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C143" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="144">
@@ -2291,10 +2291,10 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C144" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="145">
@@ -2304,10 +2304,10 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C145" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="146">
@@ -2317,10 +2317,10 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C146" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="147">
@@ -2330,10 +2330,10 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C147" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="148">
@@ -2343,10 +2343,10 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C148" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="149">
@@ -2356,10 +2356,10 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C149" t="n">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="150">
@@ -2369,10 +2369,10 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C150" t="n">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="151">
@@ -2382,10 +2382,10 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C151" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="152">
@@ -2395,10 +2395,10 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C152" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="153">
@@ -2408,10 +2408,10 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C153" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="154">
@@ -2421,10 +2421,10 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C154" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="155">
@@ -2437,7 +2437,7 @@
         <v>551</v>
       </c>
       <c r="C155" t="n">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="156">
@@ -2447,10 +2447,10 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C156" t="n">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="157">
@@ -2460,10 +2460,10 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C157" t="n">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="158">
@@ -2473,10 +2473,10 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C158" t="n">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="159">
@@ -2486,10 +2486,10 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C159" t="n">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="160">
@@ -2499,10 +2499,10 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C160" t="n">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="161">
@@ -2512,10 +2512,10 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C161" t="n">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="162">
@@ -2525,10 +2525,10 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C162" t="n">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="163">
@@ -2538,10 +2538,10 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C163" t="n">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="164">
@@ -2551,10 +2551,10 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C164" t="n">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="165">
@@ -2564,10 +2564,10 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C165" t="n">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="166">
@@ -2577,10 +2577,10 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C166" t="n">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="167">
@@ -2590,10 +2590,10 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C167" t="n">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="168">
@@ -2606,7 +2606,7 @@
         <v>552</v>
       </c>
       <c r="C168" t="n">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="169">
@@ -2616,10 +2616,10 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C169" t="n">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="170">
@@ -2629,10 +2629,10 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C170" t="n">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="171">
@@ -2642,10 +2642,10 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C171" t="n">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="172">
@@ -2655,10 +2655,10 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C172" t="n">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="173">
@@ -2668,10 +2668,10 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C173" t="n">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="174">
@@ -2681,10 +2681,10 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C174" t="n">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="175">
@@ -2694,10 +2694,10 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C175" t="n">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="176">
@@ -2707,10 +2707,10 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="C176" t="n">
-        <v>567</v>
+        <v>588</v>
       </c>
     </row>
     <row r="177">
@@ -2723,7 +2723,7 @@
         <v>548</v>
       </c>
       <c r="C177" t="n">
-        <v>527</v>
+        <v>570</v>
       </c>
     </row>
     <row r="178">
@@ -2733,10 +2733,10 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="C178" t="n">
-        <v>480</v>
+        <v>530</v>
       </c>
     </row>
     <row r="179">
@@ -2746,10 +2746,10 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="C179" t="n">
-        <v>433</v>
+        <v>481</v>
       </c>
     </row>
     <row r="180">
@@ -2759,10 +2759,10 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>579</v>
+        <v>561</v>
       </c>
       <c r="C180" t="n">
-        <v>385</v>
+        <v>436</v>
       </c>
     </row>
     <row r="181">
@@ -2772,10 +2772,10 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>600</v>
+        <v>578</v>
       </c>
       <c r="C181" t="n">
-        <v>339</v>
+        <v>389</v>
       </c>
     </row>
     <row r="182">
@@ -2785,10 +2785,10 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>628</v>
+        <v>600</v>
       </c>
       <c r="C182" t="n">
-        <v>298</v>
+        <v>341</v>
       </c>
     </row>
     <row r="183">
@@ -2798,10 +2798,10 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>663</v>
+        <v>627</v>
       </c>
       <c r="C183" t="n">
-        <v>258</v>
+        <v>300</v>
       </c>
     </row>
     <row r="184">
@@ -2811,10 +2811,10 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>700</v>
+        <v>661</v>
       </c>
       <c r="C184" t="n">
-        <v>226</v>
+        <v>262</v>
       </c>
     </row>
     <row r="185">
@@ -2824,10 +2824,10 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>743</v>
+        <v>700</v>
       </c>
       <c r="C185" t="n">
-        <v>200</v>
+        <v>229</v>
       </c>
     </row>
     <row r="186">
@@ -2837,10 +2837,10 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>788</v>
+        <v>741</v>
       </c>
       <c r="C186" t="n">
-        <v>181</v>
+        <v>202</v>
       </c>
     </row>
     <row r="187">
@@ -2850,10 +2850,10 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>836</v>
+        <v>786</v>
       </c>
       <c r="C187" t="n">
-        <v>168</v>
+        <v>183</v>
       </c>
     </row>
     <row r="188">
@@ -2863,10 +2863,10 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>884</v>
+        <v>835</v>
       </c>
       <c r="C188" t="n">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="189">
@@ -2876,7 +2876,7 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>934</v>
+        <v>884</v>
       </c>
       <c r="C189" t="n">
         <v>165</v>
@@ -2889,10 +2889,10 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>983</v>
+        <v>933</v>
       </c>
       <c r="C190" t="n">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="191">
@@ -2902,10 +2902,10 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>1032</v>
+        <v>982</v>
       </c>
       <c r="C191" t="n">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="192">
@@ -2915,10 +2915,10 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>1076</v>
+        <v>1030</v>
       </c>
       <c r="C192" t="n">
-        <v>220</v>
+        <v>195</v>
       </c>
     </row>
     <row r="193">
@@ -2928,10 +2928,10 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>1117</v>
+        <v>1074</v>
       </c>
       <c r="C193" t="n">
-        <v>252</v>
+        <v>220</v>
       </c>
     </row>
     <row r="194">
@@ -2941,10 +2941,10 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>1154</v>
+        <v>1115</v>
       </c>
       <c r="C194" t="n">
-        <v>288</v>
+        <v>253</v>
       </c>
     </row>
     <row r="195">
@@ -2954,10 +2954,10 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>1186</v>
+        <v>1153</v>
       </c>
       <c r="C195" t="n">
-        <v>331</v>
+        <v>290</v>
       </c>
     </row>
     <row r="196">
@@ -2967,10 +2967,10 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>1208</v>
+        <v>1185</v>
       </c>
       <c r="C196" t="n">
-        <v>371</v>
+        <v>333</v>
       </c>
     </row>
     <row r="197">
@@ -2980,10 +2980,10 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="C197" t="n">
-        <v>390</v>
+        <v>373</v>
       </c>
     </row>
     <row r="198">
@@ -2993,10 +2993,10 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="C198" t="n">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="199">
@@ -3006,10 +3006,10 @@
         </is>
       </c>
       <c r="B199" t="n">
-        <v>1239</v>
+        <v>1211</v>
       </c>
       <c r="C199" t="n">
-        <v>428</v>
+        <v>396</v>
       </c>
     </row>
     <row r="200">
@@ -3019,10 +3019,10 @@
         </is>
       </c>
       <c r="B200" t="n">
-        <v>1266</v>
+        <v>1238</v>
       </c>
       <c r="C200" t="n">
-        <v>463</v>
+        <v>429</v>
       </c>
     </row>
     <row r="201">
@@ -3032,10 +3032,10 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>1287</v>
+        <v>1265</v>
       </c>
       <c r="C201" t="n">
-        <v>499</v>
+        <v>465</v>
       </c>
     </row>
     <row r="202">
@@ -3045,10 +3045,10 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="C202" t="n">
-        <v>539</v>
+        <v>500</v>
       </c>
     </row>
     <row r="203">
@@ -3058,10 +3058,10 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>1317</v>
+        <v>1303</v>
       </c>
       <c r="C203" t="n">
-        <v>585</v>
+        <v>541</v>
       </c>
     </row>
     <row r="204">
@@ -3071,10 +3071,10 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>1323</v>
+        <v>1316</v>
       </c>
       <c r="C204" t="n">
-        <v>632</v>
+        <v>586</v>
       </c>
     </row>
     <row r="205">
@@ -3084,10 +3084,10 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="C205" t="n">
-        <v>675</v>
+        <v>634</v>
       </c>
     </row>
     <row r="206">
@@ -3097,10 +3097,10 @@
         </is>
       </c>
       <c r="B206" t="n">
-        <v>1301</v>
+        <v>1322</v>
       </c>
       <c r="C206" t="n">
-        <v>671</v>
+        <v>676</v>
       </c>
     </row>
     <row r="207">
@@ -3110,10 +3110,10 @@
         </is>
       </c>
       <c r="B207" t="n">
-        <v>1271</v>
+        <v>1301</v>
       </c>
       <c r="C207" t="n">
-        <v>666</v>
+        <v>672</v>
       </c>
     </row>
     <row r="208">
@@ -3123,10 +3123,10 @@
         </is>
       </c>
       <c r="B208" t="n">
-        <v>1234</v>
+        <v>1271</v>
       </c>
       <c r="C208" t="n">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="209">
@@ -3136,10 +3136,10 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>1203</v>
+        <v>1234</v>
       </c>
       <c r="C209" t="n">
-        <v>678</v>
+        <v>669</v>
       </c>
     </row>
     <row r="210">
@@ -3149,10 +3149,10 @@
         </is>
       </c>
       <c r="B210" t="n">
-        <v>1185</v>
+        <v>1203</v>
       </c>
       <c r="C210" t="n">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="211">
@@ -3162,7 +3162,7 @@
         </is>
       </c>
       <c r="B211" t="n">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="C211" t="n">
         <v>685</v>
@@ -3175,10 +3175,10 @@
         </is>
       </c>
       <c r="B212" t="n">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C212" t="n">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="213">
@@ -3188,10 +3188,10 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="C213" t="n">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="214">
@@ -3204,7 +3204,7 @@
         <v>1183</v>
       </c>
       <c r="C214" t="n">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="215">
@@ -3214,10 +3214,10 @@
         </is>
       </c>
       <c r="B215" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C215" t="n">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="216">
@@ -3227,7 +3227,7 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C216" t="n">
         <v>685</v>
@@ -3243,7 +3243,7 @@
         <v>1183</v>
       </c>
       <c r="C217" t="n">
-        <v>684</v>
+        <v>687</v>
       </c>
     </row>
     <row r="218">
@@ -3253,10 +3253,10 @@
         </is>
       </c>
       <c r="B218" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C218" t="n">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="219">
@@ -3266,10 +3266,10 @@
         </is>
       </c>
       <c r="B219" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C219" t="n">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="220">
@@ -3279,10 +3279,10 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C220" t="n">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="221">
@@ -3295,7 +3295,7 @@
         <v>1182</v>
       </c>
       <c r="C221" t="n">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="222">
@@ -3305,10 +3305,10 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C222" t="n">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="223">
@@ -3318,10 +3318,10 @@
         </is>
       </c>
       <c r="B223" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C223" t="n">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="224">
@@ -3331,10 +3331,10 @@
         </is>
       </c>
       <c r="B224" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C224" t="n">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="225">
@@ -3344,10 +3344,10 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C225" t="n">
-        <v>684</v>
+        <v>687</v>
       </c>
     </row>
     <row r="226">
@@ -3357,10 +3357,10 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C226" t="n">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="227">
@@ -3370,10 +3370,10 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C227" t="n">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="228">
@@ -3383,10 +3383,10 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C228" t="n">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="229">
@@ -3399,7 +3399,7 @@
         <v>1182</v>
       </c>
       <c r="C229" t="n">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="230">
@@ -3412,7 +3412,7 @@
         <v>1182</v>
       </c>
       <c r="C230" t="n">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="231">
@@ -3425,7 +3425,7 @@
         <v>1182</v>
       </c>
       <c r="C231" t="n">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="232">
@@ -3435,10 +3435,10 @@
         </is>
       </c>
       <c r="B232" t="n">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C232" t="n">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="233">
@@ -3448,10 +3448,10 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C233" t="n">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="234">
@@ -3461,10 +3461,10 @@
         </is>
       </c>
       <c r="B234" t="n">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C234" t="n">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="235">
@@ -3477,7 +3477,7 @@
         <v>1182</v>
       </c>
       <c r="C235" t="n">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="236">
@@ -3487,10 +3487,10 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>1184</v>
+        <v>1181</v>
       </c>
       <c r="C236" t="n">
-        <v>680</v>
+        <v>684</v>
       </c>
     </row>
     <row r="237">
@@ -3500,10 +3500,10 @@
         </is>
       </c>
       <c r="B237" t="n">
-        <v>1207</v>
+        <v>1183</v>
       </c>
       <c r="C237" t="n">
-        <v>666</v>
+        <v>681</v>
       </c>
     </row>
     <row r="238">
@@ -3513,10 +3513,10 @@
         </is>
       </c>
       <c r="B238" t="n">
-        <v>1231</v>
+        <v>1206</v>
       </c>
       <c r="C238" t="n">
-        <v>647</v>
+        <v>667</v>
       </c>
     </row>
     <row r="239">
@@ -3526,10 +3526,10 @@
         </is>
       </c>
       <c r="B239" t="n">
-        <v>1248</v>
+        <v>1229</v>
       </c>
       <c r="C239" t="n">
-        <v>617</v>
+        <v>648</v>
       </c>
     </row>
     <row r="240">
@@ -3539,10 +3539,10 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="C240" t="n">
-        <v>566</v>
+        <v>620</v>
       </c>
     </row>
     <row r="241">
@@ -3552,10 +3552,10 @@
         </is>
       </c>
       <c r="B241" t="n">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="C241" t="n">
-        <v>522</v>
+        <v>568</v>
       </c>
     </row>
     <row r="242">
@@ -3565,10 +3565,10 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>1247</v>
+        <v>1252</v>
       </c>
       <c r="C242" t="n">
-        <v>475</v>
+        <v>525</v>
       </c>
     </row>
     <row r="243">
@@ -3578,10 +3578,10 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>1229</v>
+        <v>1245</v>
       </c>
       <c r="C243" t="n">
-        <v>424</v>
+        <v>478</v>
       </c>
     </row>
     <row r="244">
@@ -3591,10 +3591,10 @@
         </is>
       </c>
       <c r="B244" t="n">
-        <v>1208</v>
+        <v>1229</v>
       </c>
       <c r="C244" t="n">
-        <v>386</v>
+        <v>428</v>
       </c>
     </row>
     <row r="245">
@@ -3604,10 +3604,10 @@
         </is>
       </c>
       <c r="B245" t="n">
-        <v>1191</v>
+        <v>1208</v>
       </c>
       <c r="C245" t="n">
-        <v>363</v>
+        <v>388</v>
       </c>
     </row>
     <row r="246">
@@ -3617,10 +3617,10 @@
         </is>
       </c>
       <c r="B246" t="n">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="C246" t="n">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="247">
@@ -3633,7 +3633,7 @@
         <v>1191</v>
       </c>
       <c r="C247" t="n">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="248">
@@ -3646,7 +3646,7 @@
         <v>1191</v>
       </c>
       <c r="C248" t="n">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="249">
@@ -3656,10 +3656,10 @@
         </is>
       </c>
       <c r="B249" t="n">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="C249" t="n">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="250">
@@ -3669,10 +3669,10 @@
         </is>
       </c>
       <c r="B250" t="n">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C250" t="n">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="251">
@@ -3682,10 +3682,10 @@
         </is>
       </c>
       <c r="B251" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C251" t="n">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="252">
@@ -3695,10 +3695,10 @@
         </is>
       </c>
       <c r="B252" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C252" t="n">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="253">
@@ -3708,10 +3708,10 @@
         </is>
       </c>
       <c r="B253" t="n">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C253" t="n">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="254">
@@ -3721,10 +3721,10 @@
         </is>
       </c>
       <c r="B254" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C254" t="n">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="255">
@@ -3734,10 +3734,10 @@
         </is>
       </c>
       <c r="B255" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C255" t="n">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="256">
@@ -3747,10 +3747,10 @@
         </is>
       </c>
       <c r="B256" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C256" t="n">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="257">
@@ -3760,10 +3760,10 @@
         </is>
       </c>
       <c r="B257" t="n">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C257" t="n">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="258">
@@ -3776,7 +3776,7 @@
         <v>1192</v>
       </c>
       <c r="C258" t="n">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="259">
@@ -3786,10 +3786,10 @@
         </is>
       </c>
       <c r="B259" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C259" t="n">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="260">
@@ -3799,10 +3799,10 @@
         </is>
       </c>
       <c r="B260" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C260" t="n">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="261">
@@ -3812,10 +3812,10 @@
         </is>
       </c>
       <c r="B261" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C261" t="n">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="262">
@@ -3825,10 +3825,10 @@
         </is>
       </c>
       <c r="B262" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C262" t="n">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="263">
@@ -3838,10 +3838,10 @@
         </is>
       </c>
       <c r="B263" t="n">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C263" t="n">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="264">
@@ -3851,10 +3851,10 @@
         </is>
       </c>
       <c r="B264" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C264" t="n">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="265">
@@ -3864,10 +3864,10 @@
         </is>
       </c>
       <c r="B265" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C265" t="n">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="266">
@@ -3877,10 +3877,10 @@
         </is>
       </c>
       <c r="B266" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C266" t="n">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="267">
@@ -3893,7 +3893,7 @@
         <v>1192</v>
       </c>
       <c r="C267" t="n">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="268">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="B268" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C268" t="n">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="269">
@@ -3916,10 +3916,10 @@
         </is>
       </c>
       <c r="B269" t="n">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C269" t="n">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="270">
@@ -3932,7 +3932,7 @@
         <v>1192</v>
       </c>
       <c r="C270" t="n">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="271">
@@ -3942,10 +3942,10 @@
         </is>
       </c>
       <c r="B271" t="n">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C271" t="n">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="272">
@@ -3955,10 +3955,10 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C272" t="n">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="273">
@@ -3981,10 +3981,10 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C274" t="n">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row r="275">
@@ -3994,10 +3994,10 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C275" t="n">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="276">
@@ -4007,10 +4007,10 @@
         </is>
       </c>
       <c r="B276" t="n">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C276" t="n">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="277">
@@ -4020,7 +4020,7 @@
         </is>
       </c>
       <c r="B277" t="n">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C277" t="n">
         <v>366</v>
@@ -4033,7 +4033,7 @@
         </is>
       </c>
       <c r="B278" t="n">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C278" t="n">
         <v>367</v>
@@ -4046,10 +4046,23 @@
         </is>
       </c>
       <c r="B279" t="n">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C279" t="n">
-        <v>369</v>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Frame 280</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>1192</v>
+      </c>
+      <c r="C280" t="n">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>